<commit_message>
added more short form street types to constants; made some fixes to tagger ground truth files; re-ran master file
</commit_message>
<xml_diff>
--- a/data/tagged stnd CO Stores - hwy as street type.xlsx
+++ b/data/tagged stnd CO Stores - hwy as street type.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\GitHub\CS410-Project\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
@@ -4459,9 +4464,6 @@
     <t>COUNTY ROAD</t>
   </si>
   <si>
-    <t>U.S. 85 87</t>
-  </si>
-  <si>
     <t>INTERSTATE</t>
   </si>
   <si>
@@ -4526,6 +4528,9 @@
   </si>
   <si>
     <t>B B</t>
+  </si>
+  <si>
+    <t>U.S 85 87</t>
   </si>
 </sst>
 </file>
@@ -4653,7 +4658,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4688,7 +4693,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4903,8 +4908,8 @@
   <dimension ref="A1:L507"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A350" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L500" sqref="L500"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H505" sqref="H505"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5764,7 +5769,7 @@
         <v>740</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -5857,10 +5862,10 @@
         <v>688</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
     </row>
     <row r="33" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -6756,7 +6761,7 @@
         <v>680</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="64" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -6953,7 +6958,7 @@
         <v>813</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>1480</v>
+        <v>1502</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>674</v>
@@ -7095,7 +7100,7 @@
         <v>25</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="76" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -7469,7 +7474,7 @@
         <v>740</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="89" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -8194,7 +8199,7 @@
         <v>680</v>
       </c>
       <c r="L113" s="1" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="114" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -8435,7 +8440,7 @@
         <v>710</v>
       </c>
       <c r="L121" s="1" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
     </row>
     <row r="122" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -8931,7 +8936,7 @@
         <v>740</v>
       </c>
       <c r="L138" s="1" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="139" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -10769,7 +10774,7 @@
         <v>1012</v>
       </c>
       <c r="H202" s="1" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="I202" s="1" t="s">
         <v>674</v>
@@ -11557,7 +11562,7 @@
         <v>1050</v>
       </c>
       <c r="H230" s="1" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="I230" s="1" t="s">
         <v>674</v>
@@ -12321,10 +12326,10 @@
         <v>677</v>
       </c>
       <c r="K255" s="1" t="s">
+        <v>1492</v>
+      </c>
+      <c r="L255" s="1" t="s">
         <v>1493</v>
-      </c>
-      <c r="L255" s="1" t="s">
-        <v>1494</v>
       </c>
     </row>
     <row r="256" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -12402,7 +12407,7 @@
         <v>1071</v>
       </c>
       <c r="H258" s="1" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="I258" s="1" t="s">
         <v>674</v>
@@ -13530,7 +13535,7 @@
         <v>740</v>
       </c>
       <c r="L297" s="1" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
     </row>
     <row r="298" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -14179,7 +14184,7 @@
         <v>1168</v>
       </c>
       <c r="L320" s="1" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
     </row>
     <row r="321" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -14722,7 +14727,7 @@
         <v>1168</v>
       </c>
       <c r="L338" s="1" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="339" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -15723,7 +15728,7 @@
         <v>740</v>
       </c>
       <c r="L372" s="1" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
     </row>
     <row r="373" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -16016,7 +16021,7 @@
         <v>740</v>
       </c>
       <c r="L382" s="1" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="383" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -16277,7 +16282,7 @@
         <v>1257</v>
       </c>
       <c r="H391" s="1" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="I391" s="1" t="s">
         <v>674</v>
@@ -16637,7 +16642,7 @@
         <v>680</v>
       </c>
       <c r="L403" s="1" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="404" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -16689,7 +16694,7 @@
         <v>25</v>
       </c>
       <c r="I405" s="1" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="406" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -16863,7 +16868,7 @@
         <v>740</v>
       </c>
       <c r="L411" s="1" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="412" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -17321,7 +17326,7 @@
         <v>25</v>
       </c>
       <c r="I427" s="1" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="428" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -17408,7 +17413,7 @@
         <v>677</v>
       </c>
       <c r="L430" s="1" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="431" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -17440,7 +17445,7 @@
         <v>1168</v>
       </c>
       <c r="L431" s="1" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="432" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -17872,7 +17877,7 @@
         <v>1168</v>
       </c>
       <c r="L446" s="1" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="447" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -18321,7 +18326,7 @@
         <v>725</v>
       </c>
       <c r="L462" s="1" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="463" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -19409,7 +19414,7 @@
         <v>1168</v>
       </c>
       <c r="L499" s="1" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="500" spans="1:12" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">

</xml_diff>